<commit_message>
updated controlled variables, protocol description, PI, PI Algo, fixed typos
</commit_message>
<xml_diff>
--- a/data/beast/beast-v3.xlsx
+++ b/data/beast/beast-v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="194">
   <si>
     <t xml:space="preserve">Scenario-Protocol-PI-PI Algo template</t>
   </si>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Definition</t>
   </si>
   <si>
-    <t xml:space="preserve">In its trolley version, the protocol evaluates the capability of the robot to safely and accurately operate a self-supporting wheeled transport device (the trolley) while performing navigation tasks.In its walker version, aimed at scenarios where the main difficulty lies in the walking process itself, the protocol evaluates the capability of the robot to minimise its reliance on an external stability-supporting device (the walker).</t>
+    <t xml:space="preserve">In its trolley version, the protocol evaluates the capability of the robot to safely and accurately operate a self-supporting wheeled transport device (the trolley) while performing navigation tasks. In its walker version, aimed at scenarios where the main difficulty lies in the walking process itself, the protocol evaluates the capability of the robot to minimise its reliance on an external stability-supporting device (the walker).</t>
   </si>
   <si>
     <t xml:space="preserve">Paragraph indicating the purpose, objective of the protocol. What are we characterising, how do we characterise it?</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">Suitable Bipedal Systems</t>
   </si>
   <si>
-    <t xml:space="preserve">Developed for humanoid; suitabile also for prosthesis, exoskeleton, human</t>
+    <t xml:space="preserve">Developed for humanoid; suitable also for prosthesis, exoskeleton, human</t>
   </si>
   <si>
     <t xml:space="preserve">Possible values: Humanoid, prosthesis, exoskeleton, human (can be various)</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">enum</t>
   </si>
   <si>
-    <t xml:space="preserve">To be defined</t>
+    <t xml:space="preserve">[0, 9000]</t>
   </si>
   <si>
     <t xml:space="preserve">grams</t>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve">The profile of breaking action applied to the door panel based on its angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[No Force, Sudden Force]</t>
   </si>
   <si>
     <t xml:space="preserve">Testbed</t>
@@ -318,25 +321,19 @@
     <t xml:space="preserve">Navigate to Checkpoint 1</t>
   </si>
   <si>
-    <t xml:space="preserve">See link below for checkpoint definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive trolley/walker to checkpoint 2 with minimum deviation from a straight trajectory, avoiding collisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive trolley/walker to checkpoint 3 and then to checkpoint 4, keeping the nearest blue obstacle on the right and avoiding collisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive trolley/walker to checkpoint 5, keeping the red obstacle on the left and avoiding collisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drive trolley/walker to checkpoint 6 and then to checkpoint 7, keeping the nearest blue obstacle on the right and avoiding collisions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(wait for benchmark [automatic] completion)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/docs/blob/master/beast_performance_indicators_and_preprocessed_data.md/</t>
+    <t xml:space="preserve">Navigate to Checkpoint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to Checkpoint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to Checkpoint 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigate to Checkpoint 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(wait for benchmark completion)</t>
   </si>
   <si>
     <t xml:space="preserve">Does your protocol involve several runs?</t>
@@ -367,7 +364,7 @@
     <t xml:space="preserve">Can your protocol involves several subjects</t>
   </si>
   <si>
-    <t xml:space="preserve">This only makes sense for protocols involving human subjects. This is a common practice to involve several huamn subjects when conducting an experimentation.</t>
+    <t xml:space="preserve">This only makes sense for protocols involving human subjects. This is a common practice to involve several human subjects when conducting an experimentation.</t>
   </si>
   <si>
     <t xml:space="preserve">Performance Indicator (PI)</t>
@@ -376,10 +373,10 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">Overall execution time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall duration of benchmark execution.</t>
+    <t xml:space="preserve">Time to grip handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from the start of the benchmark to the first time the handle is touched by the robot/humanoid. This PI accounts for the time the robot takes to perceive the walker/trolley's handle, plan its actions and grasp the handle.</t>
   </si>
   <si>
     <t xml:space="preserve">seconds</t>
@@ -423,46 +420,61 @@
   </si>
   <si>
     <t xml:space="preserve">Average of score for all subjects should be fine.
-The score may be very dependant on the subject, so we advise to run the experiments with the same subjects.</t>
+The score may be very dependent on the subject, so we advise to run the experiments with the same subjects.</t>
   </si>
   <si>
     <t xml:space="preserve">Only relevant for protocols involving human subjects. We would get a score per subject: how do we generate a global score across all subjects?</t>
   </si>
   <si>
-    <t xml:space="preserve">Time to handle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time elapsed from the start of the benchmark to the first time the handle is touched by the robot/humanoid. This PI accounts for the time the robot takes to perceive the walker/trolley's handle, plan its actions and grasp the handle.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Straight time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time elapsed on the straight segment between checkpoint 1 and checkpoint 2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slalom time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time elapsed on the slalom segments between checkpoint 2 and checkpoint 7.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Straight control accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This PI is a measurement of the accuracy of controlling the walker/trolley by the humanoid based on the trajectory of the walker/trolley on the straight segment.</t>
+    <t xml:space="preserve">Time to checkpoint 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from when the trolley/walker starts moving to when the trolley/walker crosses the checkpoint 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to checkpoint 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from when the trolley/walker starts moving to when the trolley/walker crosses the checkpoint 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to checkpoint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from when the trolley/walker starts moving to when the trolley/walker crosses the checkpoint 3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to checkpoint 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from when the trolley/walker starts moving to when the trolley/walker crosses the checkpoint 4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to checkpoint 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time elapsed from when the trolley/walker starts moving to when the trolley/walker crosses the checkpoint 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roughness of actuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum force applied to the handle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety of navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This PI is a measurement of the safety of the navigation. It is obtained as the minimum distance of the walker/trolley from the obstacles.</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">[[0, mean], [0, median], [0, std], [min, 0], [max, 0]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Safety of navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This PI is a measurement of the safety of the navigation. It is obtained as the minimum distance of the walker/trolley from the obstacles.</t>
   </si>
   <si>
     <t xml:space="preserve">Capability level</t>
@@ -481,10 +493,10 @@
     <t xml:space="preserve">Algorithm name</t>
   </si>
   <si>
-    <t xml:space="preserve">overall_execution_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difference between time of events from the ‘events sequence’ timeseries.</t>
+    <t xml:space="preserve">beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute all metrics related to beast protocol</t>
   </si>
   <si>
     <t xml:space="preserve">Url paper</t>
@@ -493,31 +505,37 @@
     <t xml:space="preserve">Url code</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/execution_time.py</t>
+    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Docker host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurobenchtest</t>
   </si>
   <si>
     <t xml:space="preserve">Docker image</t>
   </si>
   <si>
-    <t xml:space="preserve">TBD</t>
+    <t xml:space="preserve">pi_madrob_beast:0.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">Associated PI</t>
   </si>
   <si>
-    <t xml:space="preserve">[Overall execution time]</t>
+    <t xml:space="preserve">[ capability_level, safety_of_navigation, roughness_of_actuation, time_to_grip_handle, time_to_checkpoint_1, time_to_checkpoint_2, time_to_checkpoint_3, time_to_checkpoint_4, time_to_checkpoint_5]</t>
   </si>
   <si>
     <t xml:space="preserve">Input files</t>
   </si>
   <si>
-    <t xml:space="preserve">[events_sequence.csv, testbed_config.yaml]</t>
+    <t xml:space="preserve">[event.csv, distance.csv, wrench.csv, condition.yaml]</t>
   </si>
   <si>
     <t xml:space="preserve">Input command</t>
   </si>
   <si>
-    <t xml:space="preserve">./overall_execution_time.py events_sequence.csv testbed_config.yaml output_dir</t>
+    <t xml:space="preserve">[run_beast, event.csv, distance.csv, wrench.csv, condition.yaml]</t>
   </si>
   <si>
     <t xml:space="preserve">Programming Language</t>
@@ -529,7 +547,7 @@
     <t xml:space="preserve">Operating System</t>
   </si>
   <si>
-    <t xml:space="preserve">Linux/Ubuntu 16.04</t>
+    <t xml:space="preserve">Linux/Ubuntu 18.04</t>
   </si>
   <si>
     <t xml:space="preserve">Version Control System</t>
@@ -553,94 +571,7 @@
     <t xml:space="preserve">Expected delivery time</t>
   </si>
   <si>
-    <t xml:space="preserve">Not available yet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_to_handle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/time_to_handle.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Time to handle]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./time_to_handle.py  events_sequence.csv testbed_config.yaml output_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">straight_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/straight_time.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Straight time]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./straight_time.py events_sequence.csv testbed_config.yaml output_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slalom_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/slalom_time.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Slalom time]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./slalom_time.py events_sequence.csv testbed_config.yaml output_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">straight_control_accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area between the trajectory of the walker/trolley and the Least Squares Regression Line fitted to the trajectory points.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/straight_control_accuracy.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Straight control accuracy]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[pose.csv]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./straight_control_accuracy.py pose.csv output_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">safety_of_navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min(r), for each value of obstacle distance r from the obstacle_distance timeseries.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/safety_of_navigation.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Safety of navigation]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[obstacle_distance.csv]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./safety_of_navigation.py obstacle_distance.csv output_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capability_level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of steps of the benchmark procedure actually completed by the robot.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/capability_level.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Capability Level]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./capability_level.py events_sequence.csv testbed_config.yaml output_dir</t>
+    <t xml:space="preserve">Already available</t>
   </si>
   <si>
     <t xml:space="preserve">Additional information related to the code used for data collection in the facility</t>
@@ -709,7 +640,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -802,6 +733,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -810,30 +747,61 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF24292E"/>
-      <name val="-apple-system"/>
-      <family val="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF24292E"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -888,8 +856,14 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFB7B7B7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -946,6 +920,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -972,7 +953,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1198,6 +1179,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1213,79 +1198,107 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1340,7 +1353,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFA4C2F4"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -2728,8 +2741,8 @@
   </sheetPr>
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2737,7 +2750,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="74.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.43"/>
@@ -2901,7 +2915,7 @@
       <c r="F13" s="16"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15"/>
       <c r="B14" s="17" t="s">
         <v>20</v>
@@ -2918,7 +2932,7 @@
       <c r="K14" s="14"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15"/>
       <c r="B15" s="17" t="s">
         <v>23</v>
@@ -2934,7 +2948,7 @@
       </c>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15"/>
       <c r="B16" s="17" t="s">
         <v>14</v>
@@ -2962,7 +2976,7 @@
       <c r="S16" s="21"/>
       <c r="T16" s="21"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>28</v>
@@ -2975,7 +2989,7 @@
       <c r="F17" s="18"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15"/>
       <c r="B18" s="12" t="s">
         <v>30</v>
@@ -2991,7 +3005,7 @@
       </c>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15"/>
       <c r="B19" s="12" t="s">
         <v>33</v>
@@ -3004,7 +3018,7 @@
       <c r="F19" s="18"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15"/>
       <c r="B20" s="12" t="s">
         <v>35</v>
@@ -3047,7 +3061,7 @@
       </c>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15"/>
       <c r="B23" s="24" t="s">
         <v>41</v>
@@ -3066,7 +3080,7 @@
       </c>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
@@ -3085,7 +3099,7 @@
       </c>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15"/>
       <c r="B25" s="12" t="s">
         <v>50</v>
@@ -3104,7 +3118,7 @@
       </c>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15"/>
       <c r="B26" s="12" t="s">
         <v>55</v>
@@ -3116,7 +3130,7 @@
         <v>52</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>45</v>
@@ -3132,39 +3146,39 @@
       <c r="F27" s="3"/>
       <c r="N27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
       <c r="J28" s="29"/>
       <c r="N28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26"/>
       <c r="B29" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
@@ -3174,16 +3188,16 @@
       <c r="J29" s="29"/>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26"/>
       <c r="B30" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="30" t="s">
         <v>64</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>63</v>
       </c>
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
@@ -3193,16 +3207,16 @@
       <c r="J30" s="29"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26"/>
       <c r="B31" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="30" t="s">
-        <v>65</v>
-      </c>
       <c r="D31" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
@@ -3212,7 +3226,7 @@
       <c r="J31" s="29"/>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26"/>
       <c r="B32" s="30"/>
       <c r="C32" s="30"/>
@@ -3225,7 +3239,7 @@
       <c r="J32" s="29"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -3265,21 +3279,21 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C36" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="40"/>
@@ -3292,28 +3306,28 @@
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="36"/>
       <c r="B37" s="37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E37" s="41"/>
       <c r="F37" s="41"/>
       <c r="G37" s="40"/>
       <c r="H37" s="42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I37" s="43" t="s">
         <v>6</v>
       </c>
       <c r="J37" s="43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K37" s="44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L37" s="44"/>
       <c r="M37" s="44"/>
@@ -3321,26 +3335,26 @@
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="36"/>
       <c r="B38" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="40"/>
       <c r="H38" s="42"/>
       <c r="I38" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="J38" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="J38" s="45" t="s">
-        <v>65</v>
-      </c>
       <c r="K38" s="45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L38" s="45"/>
       <c r="M38" s="45"/>
@@ -3397,13 +3411,13 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="36"/>
       <c r="B42" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D42" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
@@ -3419,13 +3433,13 @@
     <row r="43" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="36"/>
       <c r="B43" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38"/>
@@ -3505,13 +3519,13 @@
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="36"/>
       <c r="B48" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="38" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38"/>
@@ -3527,13 +3541,13 @@
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="36"/>
       <c r="B49" s="37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38"/>
@@ -3646,158 +3660,148 @@
     </row>
     <row r="57" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D57" s="31"/>
       <c r="E57" s="31"/>
       <c r="F57" s="31"/>
       <c r="G57" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="15"/>
       <c r="B58" s="52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" s="52" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E58" s="16"/>
       <c r="F58" s="16"/>
       <c r="N58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="15"/>
       <c r="B59" s="53" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="54" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E59" s="13"/>
       <c r="F59" s="13"/>
       <c r="N59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15"/>
       <c r="B60" s="53" t="n">
         <v>1</v>
       </c>
       <c r="C60" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>86</v>
       </c>
       <c r="E60" s="13"/>
       <c r="F60" s="13"/>
       <c r="N60" s="8"/>
     </row>
-    <row r="61" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="15"/>
       <c r="B61" s="53" t="n">
         <v>2</v>
       </c>
       <c r="C61" s="54" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="N61" s="8"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15"/>
       <c r="B62" s="53" t="n">
         <v>3</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D62" s="13" t="s">
         <v>91</v>
       </c>
+      <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
       <c r="N62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15"/>
       <c r="B63" s="53" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D63" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="D63" s="13"/>
       <c r="E63" s="13"/>
       <c r="F63" s="13"/>
       <c r="N63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15"/>
       <c r="B64" s="53" t="n">
         <v>5</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="D64" s="13"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13"/>
       <c r="N64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15"/>
       <c r="B65" s="53" t="n">
         <v>6</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D65" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="D65" s="13"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13"/>
       <c r="N65" s="8"/>
     </row>
-    <row r="66" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="15"/>
       <c r="B66" s="53" t="n">
         <v>7</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="D66" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13"/>
       <c r="N66" s="8"/>
     </row>
-    <row r="67" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="15"/>
       <c r="B67" s="53" t="n">
         <v>8</v>
@@ -3806,70 +3810,68 @@
         <v>96</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
       <c r="N67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="56" t="s">
-        <v>97</v>
-      </c>
+      <c r="B68" s="57"/>
       <c r="N68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="N69" s="8"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="57" t="s">
+    <row r="70" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="58"/>
+      <c r="C70" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B70" s="57"/>
-      <c r="C70" s="58" t="s">
+      <c r="D70" s="31" t="s">
         <v>99</v>
-      </c>
-      <c r="D70" s="31" t="s">
-        <v>100</v>
       </c>
       <c r="E70" s="31"/>
       <c r="F70" s="31"/>
       <c r="G70" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N70" s="8"/>
+    </row>
+    <row r="71" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="N70" s="8"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="59" t="s">
+      <c r="B71" s="60"/>
+      <c r="C71" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B71" s="59"/>
-      <c r="C71" s="31" t="s">
+      <c r="D71" s="31" t="s">
         <v>103</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>104</v>
       </c>
       <c r="E71" s="31"/>
       <c r="F71" s="31"/>
       <c r="G71" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="N71" s="8"/>
+    </row>
+    <row r="72" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="N71" s="8"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="59"/>
+      <c r="B72" s="60"/>
       <c r="C72" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D72" s="33"/>
       <c r="E72" s="33"/>
       <c r="F72" s="33"/>
       <c r="G72" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N72" s="8"/>
     </row>
@@ -4892,7 +4894,6 @@
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" display="https://raw.githubusercontent.com/madrob-beast/docs/master/img/beast_arena_checkpoints.png/"/>
     <hyperlink ref="D37" r:id="rId2" display="https://www.slamtec.com/en/Lidar/A3/"/>
-    <hyperlink ref="B68" r:id="rId3" display="https://github.com/madrob-beast/docs/blob/master/beast_performance_indicators_and_preprocessed_data.md/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4909,2508 +4910,1090 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N213"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="61" width="73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="61" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="61" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="61" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="62"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="60"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="B4" s="65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="70"/>
+      <c r="B13" s="70"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B14" s="63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B16" s="64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="64" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B28" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="64" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="B29" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="12" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="B30" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B31" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="70"/>
+      <c r="B35" s="70"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="64" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="66" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="12" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="64" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="B43" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="C43" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="14" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="69" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="63" t="s">
+      <c r="B44" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C44" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="14" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="69" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63" t="s">
+      <c r="B45" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C45" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="70"/>
+      <c r="B46" s="70"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B47" s="63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="64" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="B49" s="64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B50" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="64" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
+      <c r="B51" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="12" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="B52" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B53" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="70"/>
+      <c r="B57" s="70"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="66" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="12" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="64" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="B65" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="C65" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="14" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="69" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="63" t="s">
+      <c r="B66" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="C66" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="14" t="s">
+    </row>
+    <row r="67" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="69" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="63" t="s">
+      <c r="B67" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="C67" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="61" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="70"/>
+      <c r="B68" s="70"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B69" s="63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="64" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70" s="65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
+      <c r="B71" s="64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B72" s="64" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="64" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
+      <c r="B73" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="12" t="s">
+    </row>
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="B74" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B75" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="71" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="B83" s="64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B84" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="B85" s="66" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="12" t="s">
+    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="64" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="64" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
+      <c r="B87" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="C87" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="14" t="s">
+    </row>
+    <row r="88" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="69" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="63" t="s">
+      <c r="B88" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="C88" s="68" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="14" t="s">
+    </row>
+    <row r="89" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="69" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="63" t="s">
+      <c r="B89" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="C89" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="61" t="s">
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B91" s="63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="66" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
+    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="72" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
+      <c r="B93" s="64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B94" s="64" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="64" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
+      <c r="B95" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="12" t="s">
+    </row>
+    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
+      <c r="B96" s="64" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B97" s="64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="C98" s="68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C99" s="68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C100" s="68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="66"/>
+      <c r="B101" s="66"/>
+    </row>
+    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B102" s="73"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="66"/>
+      <c r="B103" s="66"/>
+    </row>
+    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B105" s="77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="78" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" s="78" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="61" t="s">
+    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="76" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" s="79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B109" s="76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="B110" s="78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="39.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B111" s="78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112" s="78" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="B113" s="78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B114" s="75" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" s="67" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N52" s="68"/>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B54" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="61" t="s">
+    <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="B115" s="80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="B116" s="64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B117" s="80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="B118" s="80" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B119" s="80" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="69" t="s">
+        <v>173</v>
+      </c>
+      <c r="B120" s="80" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="81"/>
+      <c r="B121" s="81"/>
+    </row>
+    <row r="123" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="82" t="s">
+        <v>175</v>
+      </c>
+      <c r="B123" s="82"/>
+      <c r="C123" s="66" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B59" s="67" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B70" s="69" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="63" t="s">
-        <v>121</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="7"/>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B83" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B86" s="70" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B92" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B94" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="12" t="s">
+      <c r="B124" s="84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C124" s="68"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="B95" s="12" t="s">
+      <c r="B125" s="67" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B96" s="12" t="s">
+      <c r="C125" s="68"/>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="B126" s="67"/>
+      <c r="C126" s="68"/>
+    </row>
+    <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="85" t="s">
+        <v>179</v>
+      </c>
+      <c r="B127" s="64" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B97" s="12" t="s">
+      <c r="C127" s="68"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="85" t="s">
+        <v>180</v>
+      </c>
+      <c r="B128" s="67" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B100" s="69" t="s">
+      <c r="C128" s="68"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="85" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B101" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B103" s="70" t="s">
+      <c r="B129" s="86" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B106" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B107" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="71"/>
-      <c r="B108" s="71"/>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B112" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-    </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B117" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B118" s="72" t="s">
+      <c r="C129" s="68"/>
+    </row>
+    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="85" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B121" s="70" t="s">
+      <c r="B130" s="80" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B123" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B124" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B125" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="73"/>
-      <c r="B126" s="73"/>
-    </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B127" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B128" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B129" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B130" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B131" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B132" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B133" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3"/>
-    </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B135" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B136" s="69" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B137" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B139" s="70" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B140" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B141" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B142" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B143" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="73"/>
-      <c r="B144" s="73"/>
-    </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B145" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B146" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B147" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B148" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B149" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B150" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B151" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="3"/>
-      <c r="B152" s="3"/>
-    </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B153" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B154" s="72" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B155" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B156" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B157" s="70" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B158" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B159" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B160" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B161" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="73"/>
-      <c r="B162" s="73"/>
-    </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B163" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B164" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B166" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B167" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B168" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B169" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="3"/>
-      <c r="B170" s="3"/>
-    </row>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B171" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B172" s="69" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B173" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B174" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B175" s="70" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B176" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B177" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B178" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B179" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B180" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B181" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B182" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B183" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B184" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B185" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B186" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="3"/>
-      <c r="B187" s="3"/>
-    </row>
-    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B188" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B189" s="69" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B190" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B191" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B192" s="70" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B193" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B194" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B195" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B196" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B197" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B198" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B199" s="12" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B200" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B201" s="12" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="B202" s="12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B203" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="74" t="s">
-        <v>198</v>
-      </c>
-      <c r="B205" s="74"/>
-      <c r="C205" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="B206" s="76" t="s">
-        <v>200</v>
-      </c>
-      <c r="C206" s="14"/>
-    </row>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="B207" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="C207" s="14"/>
-    </row>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="77" t="s">
-        <v>201</v>
-      </c>
-      <c r="B208" s="51"/>
-      <c r="C208" s="14"/>
-    </row>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="77" t="s">
-        <v>202</v>
-      </c>
-      <c r="B209" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="C209" s="14"/>
-    </row>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="77" t="s">
-        <v>203</v>
-      </c>
-      <c r="B210" s="51" t="s">
-        <v>162</v>
-      </c>
-      <c r="C210" s="14"/>
-    </row>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="B211" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="C211" s="14"/>
-    </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="77" t="s">
-        <v>167</v>
-      </c>
-      <c r="B212" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C212" s="14"/>
-    </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1014" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1016" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1017" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1018" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1019" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1020" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1021" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1022" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="C130" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A123:B123"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B86" r:id="rId1" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/execution_time.py"/>
-    <hyperlink ref="B103" r:id="rId2" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/time_to_handle.py"/>
-    <hyperlink ref="B121" r:id="rId3" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/straight_time.py"/>
-    <hyperlink ref="B139" r:id="rId4" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/slalom_time.py"/>
-    <hyperlink ref="B157" r:id="rId5" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/straight_control_accuracy.py"/>
-    <hyperlink ref="B175" r:id="rId6" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/safety_of_navigation.py"/>
-    <hyperlink ref="B192" r:id="rId7" display="https://github.com/madrob-beast/madrob_beast_pi/tree/master/madrob_beast_pi/beast/capability_level.py"/>
+    <hyperlink ref="B108" r:id="rId1" display="https://github.com/madrob-beast/madrob_beast_pi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7444,34 +6027,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="79" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
+      <c r="A1" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -7482,48 +6065,48 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>

</xml_diff>

<commit_message>
corrected Disturbance type desc (Scenario-Protocol, C26), improved protocol name and description (Scenario-Protocol, C14 and C15)
</commit_message>
<xml_diff>
--- a/data/beast/beast-v3.xlsx
+++ b/data/beast/beast-v3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">BEAST: operating wheeled devices. This protocol has two variants, employing two different active devices (trolley and walker) </t>
+    <t xml:space="preserve">BEAST: operating wheeled devices.</t>
   </si>
   <si>
     <t xml:space="preserve">Same comments. In scenario presenting single protocol, name can be similar.</t>
@@ -97,7 +97,25 @@
     <t xml:space="preserve">Definition</t>
   </si>
   <si>
-    <t xml:space="preserve">In its trolley version, the protocol evaluates the capability of the robot to safely and accurately operate a self-supporting wheeled transport device (the trolley) while performing navigation tasks. In its walker version, aimed at scenarios where the main difficulty lies in the walking process itself, the protocol evaluates the capability of the robot to minimise its reliance on an external stability-supporting device (the walker).</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">This protocol has two variants, employing two different active devices (trolley and walker). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">In its trolley version, the protocol evaluates the capability of the robot to safely and accurately operate a self-supporting wheeled transport device (the trolley) while performing navigation tasks. In its walker version, aimed at scenarios where the main difficulty lies in the walking process itself, the protocol evaluates the capability of the robot to minimise its reliance on an external stability-supporting device (the walker).</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Paragraph indicating the purpose, objective of the protocol. What are we characterising, how do we characterise it?</t>
@@ -212,7 +230,7 @@
     <t xml:space="preserve">disturbance type</t>
   </si>
   <si>
-    <t xml:space="preserve">The profile of breaking action applied to the door panel based on its angle</t>
+    <t xml:space="preserve">The type of disturbance applied to the motion of the trolley using the actuated wheels (the front wheels for the trolley and the rear wheels for the walker).</t>
   </si>
   <si>
     <t xml:space="preserve">[No Force, Sudden Force]</t>
@@ -695,6 +713,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -731,12 +755,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <u val="single"/>
@@ -1034,6 +1052,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1090,51 +1112,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1142,7 +1164,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1178,10 +1200,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1308,12 +1326,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1379,23 +1397,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,17 +2752,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:T1012"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.3"/>
@@ -2756,7 +2773,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2915,7 +2931,7 @@
       <c r="F13" s="16"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15"/>
       <c r="B14" s="17" t="s">
         <v>20</v>
@@ -2932,17 +2948,17 @@
       <c r="K14" s="14"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15"/>
       <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="14" t="s">
         <v>25</v>
       </c>
@@ -2953,28 +2969,28 @@
       <c r="B16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="15"/>
@@ -3032,8 +3048,8 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -3063,38 +3079,38 @@
     </row>
     <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15"/>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="25" t="s">
         <v>45</v>
       </c>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="25" t="s">
         <v>45</v>
       </c>
       <c r="N24" s="8"/>
@@ -3118,7 +3134,7 @@
       </c>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15"/>
       <c r="B26" s="12" t="s">
         <v>55</v>
@@ -3147,109 +3163,109 @@
       <c r="N27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29" t="s">
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
       <c r="N28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26"/>
-      <c r="B29" s="30" t="s">
+      <c r="A29" s="27"/>
+      <c r="B29" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
       <c r="N29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="26"/>
-      <c r="B30" s="32" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
       <c r="N30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26"/>
-      <c r="B31" s="30" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
       <c r="N31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="26"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
       <c r="N32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="26"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
       <c r="N33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3262,415 +3278,415 @@
       <c r="N34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
       <c r="N35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D36" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="39" t="s">
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
       <c r="N36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="36"/>
-      <c r="B37" s="37" t="s">
+      <c r="A37" s="37"/>
+      <c r="B37" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="41" t="s">
+      <c r="D37" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="42" t="s">
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="43" t="s">
+      <c r="I37" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="43" t="s">
+      <c r="J37" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="K37" s="44" t="s">
+      <c r="K37" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="44"/>
-      <c r="M37" s="44"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="36"/>
-      <c r="B38" s="37" t="s">
+      <c r="A38" s="37"/>
+      <c r="B38" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="45" t="s">
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="J38" s="45" t="s">
+      <c r="J38" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="K38" s="45" t="s">
+      <c r="K38" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="47"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="36"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="46"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="36"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="46"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="47"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="46"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="47"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37" t="s">
+      <c r="A42" s="37"/>
+      <c r="B42" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D42" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="47"/>
-      <c r="M42" s="47"/>
-      <c r="N42" s="46"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="48"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="47"/>
     </row>
     <row r="43" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37" t="s">
+      <c r="A43" s="37"/>
+      <c r="B43" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D43" s="38" t="s">
+      <c r="D43" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="41"/>
       <c r="N43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
       <c r="N44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="36"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="40"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
       <c r="N45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="40"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
       <c r="N46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="36"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="40"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="41"/>
       <c r="N47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36"/>
-      <c r="B48" s="37" t="s">
+      <c r="A48" s="37"/>
+      <c r="B48" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41"/>
+      <c r="M48" s="41"/>
       <c r="N48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="36"/>
-      <c r="B49" s="37" t="s">
+      <c r="A49" s="37"/>
+      <c r="B49" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C49" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D49" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="41"/>
       <c r="N49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="36"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="41"/>
       <c r="N50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
       <c r="N51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="36"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="40"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="41"/>
       <c r="N52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="36"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="40"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="41"/>
       <c r="N53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="41"/>
+      <c r="M54" s="41"/>
       <c r="N54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="48"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
       <c r="N55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="48"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="50"/>
+      <c r="A56" s="49"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
       <c r="N56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B57" s="51" t="s">
+      <c r="B57" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
       <c r="G57" s="14" t="s">
         <v>83</v>
       </c>
@@ -3678,10 +3694,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="15"/>
-      <c r="B58" s="52" t="s">
+      <c r="B58" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="52" t="s">
+      <c r="C58" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="16" t="s">
@@ -3693,10 +3709,10 @@
     </row>
     <row r="59" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="15"/>
-      <c r="B59" s="53" t="n">
+      <c r="B59" s="54" t="n">
         <v>0</v>
       </c>
-      <c r="C59" s="54" t="s">
+      <c r="C59" s="55" t="s">
         <v>86</v>
       </c>
       <c r="D59" s="13" t="s">
@@ -3708,10 +3724,10 @@
     </row>
     <row r="60" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15"/>
-      <c r="B60" s="53" t="n">
+      <c r="B60" s="54" t="n">
         <v>1</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="56" t="s">
         <v>88</v>
       </c>
       <c r="D60" s="13" t="s">
@@ -3723,10 +3739,10 @@
     </row>
     <row r="61" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="15"/>
-      <c r="B61" s="53" t="n">
+      <c r="B61" s="54" t="n">
         <v>2</v>
       </c>
-      <c r="C61" s="54" t="s">
+      <c r="C61" s="55" t="s">
         <v>89</v>
       </c>
       <c r="D61" s="13" t="s">
@@ -3738,7 +3754,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15"/>
-      <c r="B62" s="53" t="n">
+      <c r="B62" s="54" t="n">
         <v>3</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -3751,10 +3767,10 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="15"/>
-      <c r="B63" s="53" t="n">
+      <c r="B63" s="54" t="n">
         <v>4</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="12" t="s">
         <v>92</v>
       </c>
       <c r="D63" s="13"/>
@@ -3764,10 +3780,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="15"/>
-      <c r="B64" s="53" t="n">
+      <c r="B64" s="54" t="n">
         <v>5</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D64" s="13"/>
@@ -3777,10 +3793,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="15"/>
-      <c r="B65" s="53" t="n">
+      <c r="B65" s="54" t="n">
         <v>6</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="12" t="s">
         <v>94</v>
       </c>
       <c r="D65" s="13"/>
@@ -3790,10 +3806,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="15"/>
-      <c r="B66" s="53" t="n">
+      <c r="B66" s="54" t="n">
         <v>7</v>
       </c>
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="12" t="s">
         <v>95</v>
       </c>
       <c r="D66" s="13"/>
@@ -3803,7 +3819,7 @@
     </row>
     <row r="67" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="15"/>
-      <c r="B67" s="53" t="n">
+      <c r="B67" s="54" t="n">
         <v>8</v>
       </c>
       <c r="C67" s="12" t="s">
@@ -3831,11 +3847,11 @@
       <c r="C70" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="31" t="s">
+      <c r="D70" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
       <c r="G70" s="3" t="s">
         <v>100</v>
       </c>
@@ -3846,14 +3862,14 @@
         <v>101</v>
       </c>
       <c r="B71" s="60"/>
-      <c r="C71" s="31" t="s">
+      <c r="C71" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D71" s="31" t="s">
+      <c r="D71" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
       <c r="G71" s="14" t="s">
         <v>104</v>
       </c>
@@ -3864,12 +3880,12 @@
         <v>105</v>
       </c>
       <c r="B72" s="60"/>
-      <c r="C72" s="31" t="s">
+      <c r="C72" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="33"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
       <c r="G72" s="14" t="s">
         <v>106</v>
       </c>
@@ -4906,23 +4922,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="61" width="73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="61" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="61" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="61" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="61" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6006,24 +6022,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>